<commit_message>
QAPF map area 1a
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area3_c.xlsx
+++ b/_INTERPOLATION/area3_c.xlsx
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="AD3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="AD5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="AD6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="AD7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="AD8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="AD9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="AD10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AD11" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="AD12" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -1734,7 +1734,7 @@
         </is>
       </c>
       <c r="AD13" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="AD14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1934,7 +1934,7 @@
         </is>
       </c>
       <c r="AD15" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -2038,7 +2038,7 @@
         </is>
       </c>
       <c r="AD16" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="AD17" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="AD18" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="AD19" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -2450,7 +2450,7 @@
         </is>
       </c>
       <c r="AD20" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -2558,7 +2558,7 @@
         </is>
       </c>
       <c r="AD21" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -2658,7 +2658,7 @@
         </is>
       </c>
       <c r="AD22" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="AD23" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -2866,7 +2866,7 @@
         </is>
       </c>
       <c r="AD24" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="AD25" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="AD26" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -3178,7 +3178,7 @@
         </is>
       </c>
       <c r="AD27" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="AD28" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="AD29" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="AD30" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="AD31" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preprocessing smaller, enlarged areas
-i don't know if it is a added value to do the cluster analysis for all the smaller areas.
- doing some as an example can be nice
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area3_c.xlsx
+++ b/_INTERPOLATION/area3_c.xlsx
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="AD3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="AD5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="AD6" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="AD7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="AD8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="AD9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="AD10" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AD11" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="AD12" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -1734,7 +1734,7 @@
         </is>
       </c>
       <c r="AD13" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="AD14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -1934,7 +1934,7 @@
         </is>
       </c>
       <c r="AD15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -2038,7 +2038,7 @@
         </is>
       </c>
       <c r="AD16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -2146,7 +2146,7 @@
         </is>
       </c>
       <c r="AD17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -2250,7 +2250,7 @@
         </is>
       </c>
       <c r="AD18" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="AD19" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -2450,7 +2450,7 @@
         </is>
       </c>
       <c r="AD20" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -2558,7 +2558,7 @@
         </is>
       </c>
       <c r="AD21" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -2658,7 +2658,7 @@
         </is>
       </c>
       <c r="AD22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -2762,7 +2762,7 @@
         </is>
       </c>
       <c r="AD23" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -2866,7 +2866,7 @@
         </is>
       </c>
       <c r="AD24" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="AD25" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="AD26" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -3178,7 +3178,7 @@
         </is>
       </c>
       <c r="AD27" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="AD28" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="AD29" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="AD30" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="AD31" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>